<commit_message>
Fixed handling of JSON with embedded molfiles Started handling of FORCED parameter.
</commit_message>
<xml_diff>
--- a/ExcelTools/Test_Files/Registration test.xlsx
+++ b/ExcelTools/Test_Files/Registration test.xlsx
@@ -707,7 +707,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,6 +790,9 @@
       </c>
       <c r="L2" t="s">
         <v>22</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>